<commit_message>
21 Jan 23 some analysis added to the table-
</commit_message>
<xml_diff>
--- a/LOR Project.xlsx
+++ b/LOR Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\GIT\AURA_REFERENCE_LETTER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA0B771-6505-42F4-9000-F4857631319F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DD5CAE-6255-4F41-B36D-01603B60C807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-3360" yWindow="4755" windowWidth="20925" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographic_with_manager" sheetId="6" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="203">
   <si>
     <t>Male</t>
   </si>
@@ -667,9 +667,6 @@
   </si>
   <si>
     <t>Rad-with keen eye</t>
-  </si>
-  <si>
-    <t>Manager</t>
   </si>
   <si>
     <t>Others</t>
@@ -698,6 +695,15 @@
   </si>
   <si>
     <t>Ttest_indResult(statistic=-2.698, pvalue=0.007)</t>
+  </si>
+  <si>
+    <t>1.8064125016839552 0.0021007237217212063</t>
+  </si>
+  <si>
+    <t>1.2390656226452184 0.21671184908051383</t>
+  </si>
+  <si>
+    <t>Managerial positions</t>
   </si>
 </sst>
 </file>
@@ -1907,108 +1913,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2018,15 +1925,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2045,10 +1949,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2064,6 +1968,108 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2457,13 +2463,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505C4AF0-857C-415D-A894-319537C075A6}">
   <dimension ref="B2:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="17" max="17" width="50.7109375" customWidth="1"/>
     <col min="18" max="18" width="20.7109375" customWidth="1"/>
     <col min="22" max="22" width="33.42578125" customWidth="1"/>
   </cols>
@@ -2472,62 +2479,71 @@
       <c r="B2" s="25" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="I2">
+        <f>198/(198+826)</f>
+        <v>0.193359375</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q3">
+        <f>1036/336</f>
+        <v>3.0833333333333335</v>
+      </c>
+    </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="97"/>
-      <c r="C4" s="100" t="s">
+      <c r="B4" s="121"/>
+      <c r="C4" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="126" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="102" t="s">
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="103" t="s">
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="103"/>
-      <c r="N4" s="103"/>
-      <c r="O4" s="105"/>
+      <c r="M4" s="127"/>
+      <c r="N4" s="127"/>
+      <c r="O4" s="129"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="98"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="106" t="s">
+      <c r="B5" s="122"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="107"/>
-      <c r="F5" s="91" t="s">
+      <c r="E5" s="131"/>
+      <c r="F5" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="108"/>
-      <c r="H5" s="106" t="s">
+      <c r="G5" s="132"/>
+      <c r="H5" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="91" t="s">
+      <c r="I5" s="131"/>
+      <c r="J5" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="108"/>
-      <c r="L5" s="109" t="s">
+      <c r="K5" s="132"/>
+      <c r="L5" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="107"/>
-      <c r="N5" s="91" t="s">
+      <c r="M5" s="131"/>
+      <c r="N5" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="92"/>
+      <c r="O5" s="116"/>
     </row>
     <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="99"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="37" t="s">
         <v>6</v>
       </c>
@@ -2639,16 +2655,16 @@
       <c r="O8">
         <v>71.525096525096501</v>
       </c>
-      <c r="R8" s="129"/>
-      <c r="S8" s="122" t="s">
+      <c r="R8" s="96"/>
+      <c r="S8" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="T8" s="123" t="s">
+      <c r="T8" s="113" t="s">
         <v>188</v>
       </c>
-      <c r="U8" s="130"/>
-      <c r="V8" s="141" t="s">
-        <v>199</v>
+      <c r="U8" s="114"/>
+      <c r="V8" s="107" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
@@ -2668,15 +2684,15 @@
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
       <c r="O9" s="18"/>
-      <c r="R9" s="131"/>
-      <c r="S9" s="124"/>
-      <c r="T9" s="139" t="s">
+      <c r="R9" s="97"/>
+      <c r="S9" s="112"/>
+      <c r="T9" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="U9" s="140" t="s">
+      <c r="U9" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="V9" s="142"/>
+      <c r="V9" s="108"/>
     </row>
     <row r="10" spans="2:22" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
@@ -2713,19 +2729,19 @@
       <c r="O10" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="R10" s="125" t="s">
+      <c r="R10" s="92" t="s">
         <v>175</v>
       </c>
-      <c r="S10" s="126" t="s">
+      <c r="S10" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="T10" s="127" t="s">
+      <c r="T10" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="U10" s="132" t="s">
+      <c r="U10" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="V10" s="142"/>
+      <c r="V10" s="108"/>
     </row>
     <row r="11" spans="2:22" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
@@ -2762,20 +2778,20 @@
       <c r="O11" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="R11" s="125" t="s">
+      <c r="R11" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="S11" s="137">
+      <c r="S11" s="103">
         <v>18.379000000000001</v>
       </c>
-      <c r="T11" s="128">
+      <c r="T11" s="95">
         <v>18.181000000000001</v>
       </c>
-      <c r="U11" s="133">
+      <c r="U11" s="99">
         <v>19.323</v>
       </c>
-      <c r="V11" s="143" t="s">
-        <v>198</v>
+      <c r="V11" s="109" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2813,20 +2829,20 @@
       <c r="O12" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="R12" s="134" t="s">
+      <c r="R12" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="S12" s="138">
+      <c r="S12" s="104">
         <v>344.52699999999999</v>
       </c>
-      <c r="T12" s="135">
+      <c r="T12" s="101">
         <v>338.95299999999997</v>
       </c>
-      <c r="U12" s="136">
+      <c r="U12" s="102">
         <v>368.89299999999997</v>
       </c>
-      <c r="V12" s="144" t="s">
-        <v>200</v>
+      <c r="V12" s="110" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
@@ -2874,13 +2890,18 @@
         <v>39</v>
       </c>
       <c r="M14">
-        <v>19.6969696969696</v>
+        <f>L14/(L14+L15)</f>
+        <v>0.13356164383561644</v>
       </c>
       <c r="N14">
         <v>159</v>
       </c>
       <c r="O14">
-        <v>80.303030303030297</v>
+        <f>N14/(N14+N15)</f>
+        <v>0.21780821917808219</v>
+      </c>
+      <c r="Q14" s="35" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
@@ -2910,13 +2931,15 @@
         <v>253</v>
       </c>
       <c r="M15">
-        <v>30.7038834951456</v>
+        <f>L15/(L14+L15)</f>
+        <v>0.86643835616438358</v>
       </c>
       <c r="N15">
         <v>571</v>
       </c>
       <c r="O15">
-        <v>69.296116504854297</v>
+        <f>N15/(N14+N15)</f>
+        <v>0.78219178082191776</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
@@ -2937,7 +2960,7 @@
       <c r="N16" s="15"/>
       <c r="O16" s="18"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>106</v>
       </c>
@@ -2975,7 +2998,7 @@
         <v>67.875647668393697</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
         <v>107</v>
       </c>
@@ -3013,7 +3036,7 @@
         <v>78.735632183907995</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="23" t="s">
         <v>108</v>
       </c>
@@ -3051,9 +3074,9 @@
         <v>76.923076923076906</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="C20" s="41">
         <v>240</v>
@@ -3089,9 +3112,9 @@
         <v>71.25</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C21" s="41">
         <v>195</v>
@@ -3123,24 +3146,35 @@
         <v>62.564</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H22" s="61"/>
-    </row>
-    <row r="23" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="93" t="s">
+      <c r="L22" s="25">
+        <f>SUM(L18:L21)</f>
+        <v>233</v>
+      </c>
+      <c r="N22" s="25">
+        <f>SUM(N18:N21)</f>
+        <v>610</v>
+      </c>
+      <c r="Q22" s="35" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="94"/>
-      <c r="E23" s="95" t="s">
+      <c r="D23" s="118"/>
+      <c r="E23" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="96"/>
+      <c r="F23" s="120"/>
       <c r="G23" s="86" t="s">
         <v>187</v>
       </c>
       <c r="H23" s="42"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="51"/>
       <c r="C24" s="55" t="s">
         <v>6</v>
@@ -3160,7 +3194,7 @@
       <c r="O24" s="35"/>
       <c r="P24" s="35"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="52" t="s">
         <v>106</v>
       </c>
@@ -3182,7 +3216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="52" t="s">
         <v>107</v>
       </c>
@@ -3204,7 +3238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="52" t="s">
         <v>108</v>
       </c>
@@ -3226,9 +3260,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="52" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="C28" s="56">
         <v>196</v>
@@ -3248,7 +3282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="53" t="s">
         <v>109</v>
       </c>
@@ -3270,7 +3304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="54" t="s">
         <v>185</v>
       </c>
@@ -3278,7 +3312,7 @@
         <f>SUM(C25:C29)</f>
         <v>826</v>
       </c>
-      <c r="D30" s="121"/>
+      <c r="D30" s="91"/>
       <c r="E30" s="47">
         <f>SUM(E25:E29)</f>
         <v>198</v>
@@ -3290,11 +3324,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:G4"/>
@@ -3305,8 +3334,14 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" copies="2" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3314,7 +3349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:X80"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O14" sqref="O14:P14"/>
     </sheetView>
   </sheetViews>
@@ -3349,79 +3384,79 @@
     </row>
     <row r="3" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="110"/>
-      <c r="C4" s="112" t="s">
+      <c r="B4" s="134"/>
+      <c r="C4" s="136" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="113"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="113"/>
-      <c r="R4" s="110"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="113"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="137"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="136"/>
+      <c r="L4" s="136"/>
+      <c r="M4" s="136"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="137"/>
+      <c r="R4" s="134"/>
+      <c r="S4" s="136"/>
+      <c r="T4" s="136"/>
+      <c r="U4" s="136"/>
+      <c r="V4" s="136"/>
+      <c r="W4" s="136"/>
+      <c r="X4" s="137"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="111"/>
-      <c r="C5" s="114" t="s">
+      <c r="B5" s="135"/>
+      <c r="C5" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114" t="s">
+      <c r="D5" s="138"/>
+      <c r="E5" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="F5" s="138"/>
+      <c r="G5" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="H5" s="115" t="s">
+      <c r="H5" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="J5" s="111"/>
-      <c r="K5" s="114" t="s">
+      <c r="J5" s="135"/>
+      <c r="K5" s="138" t="s">
         <v>179</v>
       </c>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114" t="s">
+      <c r="L5" s="138"/>
+      <c r="M5" s="138" t="s">
         <v>181</v>
       </c>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114" t="s">
+      <c r="N5" s="138"/>
+      <c r="O5" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="P5" s="115" t="s">
+      <c r="P5" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="R5" s="111"/>
-      <c r="S5" s="114" t="s">
+      <c r="R5" s="135"/>
+      <c r="S5" s="138" t="s">
         <v>180</v>
       </c>
-      <c r="T5" s="114"/>
-      <c r="U5" s="114" t="s">
+      <c r="T5" s="138"/>
+      <c r="U5" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="V5" s="114"/>
-      <c r="W5" s="114" t="s">
+      <c r="V5" s="138"/>
+      <c r="W5" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="X5" s="115" t="s">
+      <c r="X5" s="139" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="111"/>
+      <c r="B6" s="135"/>
       <c r="C6" s="70" t="s">
         <v>6</v>
       </c>
@@ -3434,9 +3469,9 @@
       <c r="F6" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="114"/>
-      <c r="H6" s="115"/>
-      <c r="J6" s="111"/>
+      <c r="G6" s="138"/>
+      <c r="H6" s="139"/>
+      <c r="J6" s="135"/>
       <c r="K6" s="70" t="s">
         <v>6</v>
       </c>
@@ -3449,9 +3484,9 @@
       <c r="N6" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="114"/>
-      <c r="P6" s="115"/>
-      <c r="R6" s="111"/>
+      <c r="O6" s="138"/>
+      <c r="P6" s="139"/>
+      <c r="R6" s="135"/>
       <c r="S6" s="70" t="s">
         <v>6</v>
       </c>
@@ -3464,8 +3499,8 @@
       <c r="V6" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="W6" s="114"/>
-      <c r="X6" s="115"/>
+      <c r="W6" s="138"/>
+      <c r="X6" s="139"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="69" t="s">
@@ -3924,7 +3959,7 @@
     </row>
     <row r="14" spans="2:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="68">
         <v>11</v>
@@ -3945,7 +3980,7 @@
         <v>0.366498322339529</v>
       </c>
       <c r="J14" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -3966,7 +4001,7 @@
         <v>0.44797623632193301</v>
       </c>
       <c r="R14" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S14">
         <v>8</v>
@@ -4010,79 +4045,79 @@
       <c r="V16" s="42"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B17" s="110"/>
-      <c r="C17" s="112" t="s">
+      <c r="B17" s="134"/>
+      <c r="C17" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="113"/>
-      <c r="J17" s="110"/>
-      <c r="K17" s="112"/>
-      <c r="L17" s="112"/>
-      <c r="M17" s="112"/>
-      <c r="N17" s="112"/>
-      <c r="O17" s="112"/>
-      <c r="P17" s="113"/>
-      <c r="R17" s="110"/>
-      <c r="S17" s="112"/>
-      <c r="T17" s="112"/>
-      <c r="U17" s="112"/>
-      <c r="V17" s="112"/>
-      <c r="W17" s="112"/>
-      <c r="X17" s="113"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="136"/>
+      <c r="H17" s="137"/>
+      <c r="J17" s="134"/>
+      <c r="K17" s="136"/>
+      <c r="L17" s="136"/>
+      <c r="M17" s="136"/>
+      <c r="N17" s="136"/>
+      <c r="O17" s="136"/>
+      <c r="P17" s="137"/>
+      <c r="R17" s="134"/>
+      <c r="S17" s="136"/>
+      <c r="T17" s="136"/>
+      <c r="U17" s="136"/>
+      <c r="V17" s="136"/>
+      <c r="W17" s="136"/>
+      <c r="X17" s="137"/>
     </row>
     <row r="18" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="111"/>
-      <c r="C18" s="114" t="s">
+      <c r="B18" s="135"/>
+      <c r="C18" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114" t="s">
+      <c r="D18" s="138"/>
+      <c r="E18" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114" t="s">
+      <c r="F18" s="138"/>
+      <c r="G18" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="H18" s="115" t="s">
+      <c r="H18" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="J18" s="111"/>
-      <c r="K18" s="114" t="s">
+      <c r="J18" s="135"/>
+      <c r="K18" s="138" t="s">
         <v>179</v>
       </c>
-      <c r="L18" s="114"/>
-      <c r="M18" s="114" t="s">
+      <c r="L18" s="138"/>
+      <c r="M18" s="138" t="s">
         <v>180</v>
       </c>
-      <c r="N18" s="114"/>
-      <c r="O18" s="114" t="s">
+      <c r="N18" s="138"/>
+      <c r="O18" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="P18" s="115" t="s">
+      <c r="P18" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="R18" s="111"/>
-      <c r="S18" s="114" t="s">
-        <v>193</v>
-      </c>
-      <c r="T18" s="114"/>
-      <c r="U18" s="114" t="s">
+      <c r="R18" s="135"/>
+      <c r="S18" s="138" t="s">
+        <v>192</v>
+      </c>
+      <c r="T18" s="138"/>
+      <c r="U18" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="V18" s="114"/>
-      <c r="W18" s="114" t="s">
+      <c r="V18" s="138"/>
+      <c r="W18" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="X18" s="115" t="s">
+      <c r="X18" s="139" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="111"/>
+      <c r="B19" s="135"/>
       <c r="C19" s="70" t="s">
         <v>6</v>
       </c>
@@ -4095,9 +4130,9 @@
       <c r="F19" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="114"/>
-      <c r="H19" s="115"/>
-      <c r="J19" s="111"/>
+      <c r="G19" s="138"/>
+      <c r="H19" s="139"/>
+      <c r="J19" s="135"/>
       <c r="K19" s="70" t="s">
         <v>6</v>
       </c>
@@ -4110,9 +4145,9 @@
       <c r="N19" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="O19" s="114"/>
-      <c r="P19" s="115"/>
-      <c r="R19" s="111"/>
+      <c r="O19" s="138"/>
+      <c r="P19" s="139"/>
+      <c r="R19" s="135"/>
       <c r="S19" s="70" t="s">
         <v>6</v>
       </c>
@@ -4125,8 +4160,8 @@
       <c r="V19" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="W19" s="114"/>
-      <c r="X19" s="115"/>
+      <c r="W19" s="138"/>
+      <c r="X19" s="139"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B20" s="69" t="s">
@@ -4577,7 +4612,7 @@
     </row>
     <row r="27" spans="2:24" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C27">
         <v>8</v>
@@ -4598,7 +4633,7 @@
         <v>0.25495418104856199</v>
       </c>
       <c r="J27" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -4619,7 +4654,7 @@
         <v>0.45902297647342399</v>
       </c>
       <c r="R27" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S27">
         <v>7</v>
@@ -4665,47 +4700,47 @@
       <c r="F29" s="42"/>
     </row>
     <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B30" s="110"/>
-      <c r="C30" s="112" t="s">
+      <c r="B30" s="134"/>
+      <c r="C30" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="112"/>
-      <c r="E30" s="112"/>
-      <c r="F30" s="112"/>
-      <c r="G30" s="112"/>
-      <c r="H30" s="112"/>
-      <c r="I30" s="112"/>
-      <c r="J30" s="112"/>
-      <c r="K30" s="112"/>
-      <c r="L30" s="113"/>
+      <c r="D30" s="136"/>
+      <c r="E30" s="136"/>
+      <c r="F30" s="136"/>
+      <c r="G30" s="136"/>
+      <c r="H30" s="136"/>
+      <c r="I30" s="136"/>
+      <c r="J30" s="136"/>
+      <c r="K30" s="136"/>
+      <c r="L30" s="137"/>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B31" s="111"/>
-      <c r="C31" s="114" t="s">
+      <c r="B31" s="135"/>
+      <c r="C31" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114" t="s">
+      <c r="D31" s="138"/>
+      <c r="E31" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="F31" s="114"/>
-      <c r="G31" s="114" t="s">
+      <c r="F31" s="138"/>
+      <c r="G31" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="H31" s="114"/>
-      <c r="I31" s="114" t="s">
+      <c r="H31" s="138"/>
+      <c r="I31" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="J31" s="114"/>
-      <c r="K31" s="114" t="s">
+      <c r="J31" s="138"/>
+      <c r="K31" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="L31" s="115" t="s">
+      <c r="L31" s="139" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B32" s="111"/>
+      <c r="B32" s="135"/>
       <c r="C32" s="70" t="s">
         <v>6</v>
       </c>
@@ -4730,8 +4765,8 @@
       <c r="J32" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="K32" s="114"/>
-      <c r="L32" s="115"/>
+      <c r="K32" s="138"/>
+      <c r="L32" s="139"/>
     </row>
     <row r="33" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B33" s="69" t="s">
@@ -4952,7 +4987,7 @@
     </row>
     <row r="40" spans="2:24" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C40">
         <v>10</v>
@@ -5000,83 +5035,83 @@
       <c r="J42" s="42"/>
     </row>
     <row r="43" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B43" s="110"/>
-      <c r="C43" s="112" t="s">
+      <c r="B43" s="134"/>
+      <c r="C43" s="136" t="s">
         <v>177</v>
       </c>
-      <c r="D43" s="112"/>
-      <c r="E43" s="112"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="112"/>
-      <c r="H43" s="112"/>
-      <c r="I43" s="112"/>
-      <c r="J43" s="112"/>
-      <c r="K43" s="112"/>
-      <c r="L43" s="113"/>
-      <c r="N43" s="110"/>
-      <c r="O43" s="112" t="s">
+      <c r="D43" s="136"/>
+      <c r="E43" s="136"/>
+      <c r="F43" s="136"/>
+      <c r="G43" s="136"/>
+      <c r="H43" s="136"/>
+      <c r="I43" s="136"/>
+      <c r="J43" s="136"/>
+      <c r="K43" s="136"/>
+      <c r="L43" s="137"/>
+      <c r="N43" s="134"/>
+      <c r="O43" s="136" t="s">
         <v>178</v>
       </c>
-      <c r="P43" s="112"/>
-      <c r="Q43" s="112"/>
-      <c r="R43" s="112"/>
-      <c r="S43" s="112"/>
-      <c r="T43" s="112"/>
-      <c r="U43" s="112"/>
-      <c r="V43" s="112"/>
-      <c r="W43" s="112"/>
-      <c r="X43" s="113"/>
+      <c r="P43" s="136"/>
+      <c r="Q43" s="136"/>
+      <c r="R43" s="136"/>
+      <c r="S43" s="136"/>
+      <c r="T43" s="136"/>
+      <c r="U43" s="136"/>
+      <c r="V43" s="136"/>
+      <c r="W43" s="136"/>
+      <c r="X43" s="137"/>
     </row>
     <row r="44" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B44" s="111"/>
-      <c r="C44" s="114" t="s">
+      <c r="B44" s="135"/>
+      <c r="C44" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="114"/>
-      <c r="E44" s="114" t="s">
+      <c r="D44" s="138"/>
+      <c r="E44" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="F44" s="114"/>
-      <c r="G44" s="114" t="s">
+      <c r="F44" s="138"/>
+      <c r="G44" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="H44" s="114"/>
-      <c r="I44" s="114" t="s">
+      <c r="H44" s="138"/>
+      <c r="I44" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="J44" s="114"/>
-      <c r="K44" s="114" t="s">
+      <c r="J44" s="138"/>
+      <c r="K44" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="L44" s="115" t="s">
+      <c r="L44" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="N44" s="111"/>
-      <c r="O44" s="114" t="s">
+      <c r="N44" s="135"/>
+      <c r="O44" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="P44" s="114"/>
-      <c r="Q44" s="114" t="s">
+      <c r="P44" s="138"/>
+      <c r="Q44" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="R44" s="114"/>
-      <c r="S44" s="114" t="s">
+      <c r="R44" s="138"/>
+      <c r="S44" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="T44" s="114"/>
-      <c r="U44" s="114" t="s">
+      <c r="T44" s="138"/>
+      <c r="U44" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="V44" s="114"/>
-      <c r="W44" s="114" t="s">
+      <c r="V44" s="138"/>
+      <c r="W44" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="X44" s="115" t="s">
+      <c r="X44" s="139" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="45" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B45" s="111"/>
+      <c r="B45" s="135"/>
       <c r="C45" s="70" t="s">
         <v>6</v>
       </c>
@@ -5101,9 +5136,9 @@
       <c r="J45" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="K45" s="114"/>
-      <c r="L45" s="115"/>
-      <c r="N45" s="111"/>
+      <c r="K45" s="138"/>
+      <c r="L45" s="139"/>
+      <c r="N45" s="135"/>
       <c r="O45" s="70" t="s">
         <v>6</v>
       </c>
@@ -5128,8 +5163,8 @@
       <c r="V45" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="W45" s="114"/>
-      <c r="X45" s="115"/>
+      <c r="W45" s="138"/>
+      <c r="X45" s="139"/>
     </row>
     <row r="46" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B46" s="69" t="s">
@@ -5553,7 +5588,7 @@
     </row>
     <row r="53" spans="2:24" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -5580,7 +5615,7 @@
         <v>0</v>
       </c>
       <c r="N53" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O53">
         <v>9</v>
@@ -5627,83 +5662,83 @@
     </row>
     <row r="55" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B56" s="110"/>
-      <c r="C56" s="112" t="s">
+      <c r="B56" s="134"/>
+      <c r="C56" s="136" t="s">
         <v>184</v>
       </c>
-      <c r="D56" s="112"/>
-      <c r="E56" s="112"/>
-      <c r="F56" s="112"/>
-      <c r="G56" s="112"/>
-      <c r="H56" s="112"/>
-      <c r="I56" s="112"/>
-      <c r="J56" s="112"/>
-      <c r="K56" s="112"/>
-      <c r="L56" s="113"/>
-      <c r="N56" s="110"/>
-      <c r="O56" s="112" t="s">
-        <v>197</v>
-      </c>
-      <c r="P56" s="112"/>
-      <c r="Q56" s="112"/>
-      <c r="R56" s="112"/>
-      <c r="S56" s="112"/>
-      <c r="T56" s="112"/>
-      <c r="U56" s="112"/>
-      <c r="V56" s="112"/>
-      <c r="W56" s="112"/>
-      <c r="X56" s="113"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="136"/>
+      <c r="F56" s="136"/>
+      <c r="G56" s="136"/>
+      <c r="H56" s="136"/>
+      <c r="I56" s="136"/>
+      <c r="J56" s="136"/>
+      <c r="K56" s="136"/>
+      <c r="L56" s="137"/>
+      <c r="N56" s="134"/>
+      <c r="O56" s="136" t="s">
+        <v>196</v>
+      </c>
+      <c r="P56" s="136"/>
+      <c r="Q56" s="136"/>
+      <c r="R56" s="136"/>
+      <c r="S56" s="136"/>
+      <c r="T56" s="136"/>
+      <c r="U56" s="136"/>
+      <c r="V56" s="136"/>
+      <c r="W56" s="136"/>
+      <c r="X56" s="137"/>
     </row>
     <row r="57" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B57" s="111"/>
-      <c r="C57" s="114" t="s">
+      <c r="B57" s="135"/>
+      <c r="C57" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="114"/>
-      <c r="E57" s="114" t="s">
+      <c r="D57" s="138"/>
+      <c r="E57" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="F57" s="114"/>
-      <c r="G57" s="114" t="s">
+      <c r="F57" s="138"/>
+      <c r="G57" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="H57" s="114"/>
-      <c r="I57" s="114" t="s">
+      <c r="H57" s="138"/>
+      <c r="I57" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="J57" s="114"/>
-      <c r="K57" s="114" t="s">
+      <c r="J57" s="138"/>
+      <c r="K57" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="L57" s="115" t="s">
+      <c r="L57" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="N57" s="111"/>
-      <c r="O57" s="114" t="s">
+      <c r="N57" s="135"/>
+      <c r="O57" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="P57" s="114"/>
-      <c r="Q57" s="114" t="s">
+      <c r="P57" s="138"/>
+      <c r="Q57" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="R57" s="114"/>
-      <c r="S57" s="114" t="s">
+      <c r="R57" s="138"/>
+      <c r="S57" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="T57" s="114"/>
-      <c r="U57" s="114" t="s">
+      <c r="T57" s="138"/>
+      <c r="U57" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="V57" s="114"/>
-      <c r="W57" s="114" t="s">
+      <c r="V57" s="138"/>
+      <c r="W57" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="X57" s="115" t="s">
+      <c r="X57" s="139" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="58" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B58" s="111"/>
+      <c r="B58" s="135"/>
       <c r="C58" s="70" t="s">
         <v>6</v>
       </c>
@@ -5728,9 +5763,9 @@
       <c r="J58" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="K58" s="114"/>
-      <c r="L58" s="115"/>
-      <c r="N58" s="111"/>
+      <c r="K58" s="138"/>
+      <c r="L58" s="139"/>
+      <c r="N58" s="135"/>
       <c r="O58" s="70" t="s">
         <v>6</v>
       </c>
@@ -5755,8 +5790,8 @@
       <c r="V58" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="W58" s="114"/>
-      <c r="X58" s="115"/>
+      <c r="W58" s="138"/>
+      <c r="X58" s="139"/>
     </row>
     <row r="59" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B59" s="69" t="s">
@@ -6180,7 +6215,7 @@
     </row>
     <row r="66" spans="2:24" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -6207,7 +6242,7 @@
         <v>0</v>
       </c>
       <c r="N66" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O66">
         <v>1</v>
@@ -6256,83 +6291,83 @@
       <c r="F68" s="67"/>
     </row>
     <row r="69" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B69" s="110"/>
-      <c r="C69" s="112" t="s">
-        <v>196</v>
-      </c>
-      <c r="D69" s="112"/>
-      <c r="E69" s="112"/>
-      <c r="F69" s="112"/>
-      <c r="G69" s="112"/>
-      <c r="H69" s="112"/>
-      <c r="I69" s="112"/>
-      <c r="J69" s="112"/>
-      <c r="K69" s="112"/>
-      <c r="L69" s="113"/>
-      <c r="N69" s="110"/>
-      <c r="O69" s="112" t="s">
+      <c r="B69" s="134"/>
+      <c r="C69" s="136" t="s">
         <v>195</v>
       </c>
-      <c r="P69" s="112"/>
-      <c r="Q69" s="112"/>
-      <c r="R69" s="112"/>
-      <c r="S69" s="112"/>
-      <c r="T69" s="112"/>
-      <c r="U69" s="112"/>
-      <c r="V69" s="112"/>
-      <c r="W69" s="112"/>
-      <c r="X69" s="113"/>
+      <c r="D69" s="136"/>
+      <c r="E69" s="136"/>
+      <c r="F69" s="136"/>
+      <c r="G69" s="136"/>
+      <c r="H69" s="136"/>
+      <c r="I69" s="136"/>
+      <c r="J69" s="136"/>
+      <c r="K69" s="136"/>
+      <c r="L69" s="137"/>
+      <c r="N69" s="134"/>
+      <c r="O69" s="136" t="s">
+        <v>194</v>
+      </c>
+      <c r="P69" s="136"/>
+      <c r="Q69" s="136"/>
+      <c r="R69" s="136"/>
+      <c r="S69" s="136"/>
+      <c r="T69" s="136"/>
+      <c r="U69" s="136"/>
+      <c r="V69" s="136"/>
+      <c r="W69" s="136"/>
+      <c r="X69" s="137"/>
     </row>
     <row r="70" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B70" s="111"/>
-      <c r="C70" s="114" t="s">
+      <c r="B70" s="135"/>
+      <c r="C70" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="D70" s="114"/>
-      <c r="E70" s="114" t="s">
+      <c r="D70" s="138"/>
+      <c r="E70" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="F70" s="114"/>
-      <c r="G70" s="114" t="s">
+      <c r="F70" s="138"/>
+      <c r="G70" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="H70" s="114"/>
-      <c r="I70" s="114" t="s">
+      <c r="H70" s="138"/>
+      <c r="I70" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="J70" s="114"/>
-      <c r="K70" s="114" t="s">
+      <c r="J70" s="138"/>
+      <c r="K70" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="L70" s="115" t="s">
+      <c r="L70" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="N70" s="111"/>
-      <c r="O70" s="114" t="s">
+      <c r="N70" s="135"/>
+      <c r="O70" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="P70" s="114"/>
-      <c r="Q70" s="114" t="s">
+      <c r="P70" s="138"/>
+      <c r="Q70" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="R70" s="114"/>
-      <c r="S70" s="114" t="s">
+      <c r="R70" s="138"/>
+      <c r="S70" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="T70" s="114"/>
-      <c r="U70" s="114" t="s">
+      <c r="T70" s="138"/>
+      <c r="U70" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="V70" s="114"/>
-      <c r="W70" s="114" t="s">
+      <c r="V70" s="138"/>
+      <c r="W70" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="X70" s="115" t="s">
+      <c r="X70" s="139" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="71" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B71" s="111"/>
+      <c r="B71" s="135"/>
       <c r="C71" s="70" t="s">
         <v>6</v>
       </c>
@@ -6357,9 +6392,9 @@
       <c r="J71" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="K71" s="114"/>
-      <c r="L71" s="115"/>
-      <c r="N71" s="111"/>
+      <c r="K71" s="138"/>
+      <c r="L71" s="139"/>
+      <c r="N71" s="135"/>
       <c r="O71" s="70" t="s">
         <v>6</v>
       </c>
@@ -6384,8 +6419,8 @@
       <c r="V71" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="W71" s="114"/>
-      <c r="X71" s="115"/>
+      <c r="W71" s="138"/>
+      <c r="X71" s="139"/>
     </row>
     <row r="72" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B72" s="69" t="s">
@@ -6820,7 +6855,7 @@
       <c r="K79" s="79"/>
       <c r="L79" s="84"/>
       <c r="N79" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O79">
         <v>8</v>
@@ -6849,7 +6884,7 @@
     </row>
     <row r="80" spans="2:24" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -6878,6 +6913,82 @@
     </row>
   </sheetData>
   <mergeCells count="92">
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="K17:P17"/>
+    <mergeCell ref="R17:R19"/>
+    <mergeCell ref="S17:X17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="W18:W19"/>
+    <mergeCell ref="X18:X19"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="L31:L32"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="C30:L30"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="S4:X4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:L43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="N43:N45"/>
+    <mergeCell ref="O43:X43"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:V44"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="X44:X45"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="N56:N58"/>
+    <mergeCell ref="O56:X56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:K58"/>
+    <mergeCell ref="L57:L58"/>
+    <mergeCell ref="O57:P57"/>
+    <mergeCell ref="Q57:R57"/>
+    <mergeCell ref="S57:T57"/>
+    <mergeCell ref="U57:V57"/>
+    <mergeCell ref="W57:W58"/>
+    <mergeCell ref="X57:X58"/>
     <mergeCell ref="B69:B71"/>
     <mergeCell ref="C69:L69"/>
     <mergeCell ref="N69:N71"/>
@@ -6894,82 +7005,6 @@
     <mergeCell ref="U70:V70"/>
     <mergeCell ref="W70:W71"/>
     <mergeCell ref="X70:X71"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="N56:N58"/>
-    <mergeCell ref="O56:X56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:K58"/>
-    <mergeCell ref="L57:L58"/>
-    <mergeCell ref="O57:P57"/>
-    <mergeCell ref="Q57:R57"/>
-    <mergeCell ref="S57:T57"/>
-    <mergeCell ref="U57:V57"/>
-    <mergeCell ref="W57:W58"/>
-    <mergeCell ref="X57:X58"/>
-    <mergeCell ref="N43:N45"/>
-    <mergeCell ref="O43:X43"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:V44"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="X44:X45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:L43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:K45"/>
-    <mergeCell ref="L44:L45"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="S4:X4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="L31:L32"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="C30:L30"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="K17:P17"/>
-    <mergeCell ref="R17:R19"/>
-    <mergeCell ref="S17:X17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="W18:W19"/>
-    <mergeCell ref="X18:X19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" copies="2" r:id="rId1"/>
@@ -7806,59 +7841,59 @@
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="97"/>
-      <c r="C4" s="100" t="s">
+      <c r="B4" s="121"/>
+      <c r="C4" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="126" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="102" t="s">
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="103" t="s">
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="103"/>
-      <c r="N4" s="103"/>
-      <c r="O4" s="105"/>
+      <c r="M4" s="127"/>
+      <c r="N4" s="127"/>
+      <c r="O4" s="129"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="98"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="106" t="s">
+      <c r="B5" s="122"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="107"/>
-      <c r="F5" s="91" t="s">
+      <c r="E5" s="131"/>
+      <c r="F5" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="108"/>
-      <c r="H5" s="106" t="s">
+      <c r="G5" s="132"/>
+      <c r="H5" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="91" t="s">
+      <c r="I5" s="131"/>
+      <c r="J5" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="108"/>
-      <c r="L5" s="109" t="s">
+      <c r="K5" s="132"/>
+      <c r="L5" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="107"/>
-      <c r="N5" s="91" t="s">
+      <c r="M5" s="131"/>
+      <c r="N5" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="92"/>
+      <c r="O5" s="116"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="99"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="37" t="s">
         <v>6</v>
       </c>
@@ -8359,24 +8394,24 @@
     </row>
     <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="118" t="s">
+      <c r="C22" s="142" t="s">
         <v>188</v>
       </c>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="120"/>
+      <c r="D22" s="143"/>
+      <c r="E22" s="143"/>
+      <c r="F22" s="143"/>
+      <c r="G22" s="144"/>
       <c r="H22" s="61"/>
     </row>
     <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="116" t="s">
+      <c r="C23" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="117"/>
-      <c r="E23" s="117" t="s">
+      <c r="D23" s="141"/>
+      <c r="E23" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="117"/>
+      <c r="F23" s="141"/>
       <c r="G23" s="43" t="s">
         <v>187</v>
       </c>
@@ -8529,12 +8564,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="D4:G4"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="D5:E5"/>
@@ -8543,6 +8572,12 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="N5:O5"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="D4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" copies="2" r:id="rId1"/>

</xml_diff>

<commit_message>
22 Jan Sunday analysis- academic rank letter rank analysis - word cloud - gender length analysis
</commit_message>
<xml_diff>
--- a/LOR Project.xlsx
+++ b/LOR Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\GIT\AURA_REFERENCE_LETTER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benanakca/Workspace/GIT/AURA_REFERENCE_LETTER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA0B771-6505-42F4-9000-F4857631319F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ED8785-F868-1B40-93BE-1BFEAAA85E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographic_with_manager" sheetId="6" r:id="rId1"/>
@@ -51,41 +51,41 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
-        <t>[Yorum yazışması]
-Excel sürümünüz bu yorum yazışmasını okumanıza izin veriyor, ancak dosya daha yeni bir Excel sürümünde açılırsa, yapılan düzenlemeler kaldırılır. Daha fazla bilgi: https://go.microsoft.com/fwlink/?linkid=870924.
-Açıklama:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Grimm 2020</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
-        <t>[Yorum yazışması]
-Excel sürümünüz bu yorum yazışmasını okumanıza izin veriyor, ancak dosya daha yeni bir Excel sürümünde açılırsa, yapılan düzenlemeler kaldırılır. Daha fazla bilgi: https://go.microsoft.com/fwlink/?linkid=870924.
-Açıklama:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Grimm 2020</t>
       </text>
     </comment>
     <comment ref="C1" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
-        <t>[Yorum yazışması]
-Excel sürümünüz bu yorum yazışmasını okumanıza izin veriyor, ancak dosya daha yeni bir Excel sürümünde açılırsa, yapılan düzenlemeler kaldırılır. Daha fazla bilgi: https://go.microsoft.com/fwlink/?linkid=870924.
-Açıklama:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Messner and Shimahara 2008</t>
       </text>
     </comment>
     <comment ref="D1" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
-        <t>[Yorum yazışması]
-Excel sürümünüz bu yorum yazışmasını okumanıza izin veriyor, ancak dosya daha yeni bir Excel sürümünde açılırsa, yapılan düzenlemeler kaldırılır. Daha fazla bilgi: https://go.microsoft.com/fwlink/?linkid=870924.
-Açıklama:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Messner and Shimahara 2008</t>
       </text>
     </comment>
     <comment ref="E1" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
-        <t>[Yorum yazışması]
-Excel sürümünüz bu yorum yazışmasını okumanıza izin veriyor, ancak dosya daha yeni bir Excel sürümünde açılırsa, yapılan düzenlemeler kaldırılır. Daha fazla bilgi: https://go.microsoft.com/fwlink/?linkid=870924.
-Açıklama:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Messner and Shimahara 2008</t>
       </text>
     </comment>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="211">
   <si>
     <t>Male</t>
   </si>
@@ -698,13 +698,43 @@
   </si>
   <si>
     <t>Ttest_indResult(statistic=-2.698, pvalue=0.007)</t>
+  </si>
+  <si>
+    <t>Keen eye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letter writer academic rank </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Professor </t>
+  </si>
+  <si>
+    <t>Not Professor (unknown excluded)</t>
+  </si>
+  <si>
+    <t>prof</t>
+  </si>
+  <si>
+    <t>asso_prof</t>
+  </si>
+  <si>
+    <t>asis_prof</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>average sentence count</t>
+  </si>
+  <si>
+    <t>average word count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,8 +771,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -785,8 +821,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="71">
+  <borders count="82">
     <border>
       <left/>
       <right/>
@@ -1706,12 +1748,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1907,108 +2086,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2018,15 +2098,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2045,10 +2122,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2065,9 +2142,222 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="71" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="72" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="73" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2457,77 +2747,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505C4AF0-857C-415D-A894-319537C075A6}">
   <dimension ref="B2:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" customWidth="1"/>
-    <col min="22" max="22" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="39.5" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" customWidth="1"/>
+    <col min="22" max="22" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B2" s="25" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="97"/>
-      <c r="C4" s="100" t="s">
+    <row r="3" spans="2:22" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B4" s="111"/>
+      <c r="C4" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="116" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="102" t="s">
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="103" t="s">
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="103"/>
-      <c r="N4" s="103"/>
-      <c r="O4" s="105"/>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="98"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="106" t="s">
+      <c r="M4" s="117"/>
+      <c r="N4" s="117"/>
+      <c r="O4" s="119"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B5" s="112"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="107"/>
-      <c r="F5" s="91" t="s">
+      <c r="E5" s="121"/>
+      <c r="F5" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="108"/>
-      <c r="H5" s="106" t="s">
+      <c r="G5" s="123"/>
+      <c r="H5" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="91" t="s">
+      <c r="I5" s="121"/>
+      <c r="J5" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="108"/>
-      <c r="L5" s="109" t="s">
+      <c r="K5" s="123"/>
+      <c r="L5" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="107"/>
-      <c r="N5" s="91" t="s">
+      <c r="M5" s="121"/>
+      <c r="N5" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="92"/>
-    </row>
-    <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="99"/>
+      <c r="O5" s="129"/>
+    </row>
+    <row r="6" spans="2:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="113"/>
       <c r="C6" s="37" t="s">
         <v>6</v>
       </c>
@@ -2568,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
         <v>174</v>
       </c>
@@ -2604,7 +2894,7 @@
         <v>71.726190476190396</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B8" s="27" t="s">
         <v>173</v>
       </c>
@@ -2639,19 +2929,19 @@
       <c r="O8">
         <v>71.525096525096501</v>
       </c>
-      <c r="R8" s="129"/>
-      <c r="S8" s="122" t="s">
+      <c r="R8" s="96"/>
+      <c r="S8" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="T8" s="123" t="s">
+      <c r="T8" s="127" t="s">
         <v>188</v>
       </c>
-      <c r="U8" s="130"/>
-      <c r="V8" s="141" t="s">
+      <c r="U8" s="128"/>
+      <c r="V8" s="107" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
@@ -2668,17 +2958,17 @@
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
       <c r="O9" s="18"/>
-      <c r="R9" s="131"/>
-      <c r="S9" s="124"/>
-      <c r="T9" s="139" t="s">
+      <c r="R9" s="97"/>
+      <c r="S9" s="126"/>
+      <c r="T9" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="U9" s="140" t="s">
+      <c r="U9" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="V9" s="142"/>
-    </row>
-    <row r="10" spans="2:22" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V9" s="108"/>
+    </row>
+    <row r="10" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>175</v>
       </c>
@@ -2713,21 +3003,21 @@
       <c r="O10" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="R10" s="125" t="s">
+      <c r="R10" s="92" t="s">
         <v>175</v>
       </c>
-      <c r="S10" s="126" t="s">
+      <c r="S10" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="T10" s="127" t="s">
+      <c r="T10" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="U10" s="132" t="s">
+      <c r="U10" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="V10" s="142"/>
-    </row>
-    <row r="11" spans="2:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="V10" s="108"/>
+    </row>
+    <row r="11" spans="2:22" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="23" t="s">
         <v>172</v>
       </c>
@@ -2762,23 +3052,23 @@
       <c r="O11" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="R11" s="125" t="s">
+      <c r="R11" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="S11" s="137">
+      <c r="S11" s="103">
         <v>18.379000000000001</v>
       </c>
-      <c r="T11" s="128">
+      <c r="T11" s="95">
         <v>18.181000000000001</v>
       </c>
-      <c r="U11" s="133">
+      <c r="U11" s="99">
         <v>19.323</v>
       </c>
-      <c r="V11" s="143" t="s">
+      <c r="V11" s="109" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="2:22" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>10</v>
       </c>
@@ -2813,23 +3103,23 @@
       <c r="O12" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="R12" s="134" t="s">
+      <c r="R12" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="S12" s="138">
+      <c r="S12" s="104">
         <v>344.52699999999999</v>
       </c>
-      <c r="T12" s="135">
+      <c r="T12" s="101">
         <v>338.95299999999997</v>
       </c>
-      <c r="U12" s="136">
+      <c r="U12" s="102">
         <v>368.89299999999997</v>
       </c>
-      <c r="V12" s="144" t="s">
+      <c r="V12" s="110" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="22" t="s">
         <v>11</v>
       </c>
@@ -2847,7 +3137,7 @@
       <c r="N13" s="15"/>
       <c r="O13" s="18"/>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
         <v>1</v>
       </c>
@@ -2883,7 +3173,7 @@
         <v>80.303030303030297</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>0</v>
       </c>
@@ -2919,7 +3209,7 @@
         <v>69.296116504854297</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="22" t="s">
         <v>12</v>
       </c>
@@ -2936,8 +3226,20 @@
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
       <c r="O16" s="18"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S16" s="181" t="s">
+        <v>205</v>
+      </c>
+      <c r="T16" s="181" t="s">
+        <v>206</v>
+      </c>
+      <c r="U16" s="181" t="s">
+        <v>207</v>
+      </c>
+      <c r="V16" s="181" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
         <v>106</v>
       </c>
@@ -2974,8 +3276,23 @@
       <c r="O17">
         <v>67.875647668393697</v>
       </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="R17" s="181" t="s">
+        <v>209</v>
+      </c>
+      <c r="S17">
+        <v>10.625</v>
+      </c>
+      <c r="T17">
+        <v>10.633928571428569</v>
+      </c>
+      <c r="U17">
+        <v>12.35119047619048</v>
+      </c>
+      <c r="V17">
+        <v>10.011904761904759</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B18" s="23" t="s">
         <v>107</v>
       </c>
@@ -3012,8 +3329,23 @@
       <c r="O18">
         <v>78.735632183907995</v>
       </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="R18" s="181" t="s">
+        <v>210</v>
+      </c>
+      <c r="S18">
+        <v>204.33928571428569</v>
+      </c>
+      <c r="T18">
+        <v>199.78571428571431</v>
+      </c>
+      <c r="U18">
+        <v>237.31845238095241</v>
+      </c>
+      <c r="V18">
+        <v>181.76488095238099</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
         <v>108</v>
       </c>
@@ -3051,7 +3383,7 @@
         <v>76.923076923076906</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>191</v>
       </c>
@@ -3089,7 +3421,7 @@
         <v>71.25</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
         <v>192</v>
       </c>
@@ -3123,24 +3455,24 @@
         <v>62.564</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H22" s="61"/>
     </row>
-    <row r="23" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="93" t="s">
+    <row r="23" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="94"/>
-      <c r="E23" s="95" t="s">
+      <c r="D23" s="131"/>
+      <c r="E23" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="96"/>
+      <c r="F23" s="133"/>
       <c r="G23" s="86" t="s">
         <v>187</v>
       </c>
       <c r="H23" s="42"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B24" s="51"/>
       <c r="C24" s="55" t="s">
         <v>6</v>
@@ -3160,7 +3492,7 @@
       <c r="O24" s="35"/>
       <c r="P24" s="35"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B25" s="52" t="s">
         <v>106</v>
       </c>
@@ -3182,7 +3514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B26" s="52" t="s">
         <v>107</v>
       </c>
@@ -3204,7 +3536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B27" s="52" t="s">
         <v>108</v>
       </c>
@@ -3226,7 +3558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B28" s="52" t="s">
         <v>191</v>
       </c>
@@ -3248,7 +3580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B29" s="53" t="s">
         <v>109</v>
       </c>
@@ -3270,7 +3602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="54" t="s">
         <v>185</v>
       </c>
@@ -3278,7 +3610,7 @@
         <f>SUM(C25:C29)</f>
         <v>826</v>
       </c>
-      <c r="D30" s="121"/>
+      <c r="D30" s="91"/>
       <c r="E30" s="47">
         <f>SUM(E25:E29)</f>
         <v>198</v>
@@ -3312,116 +3644,116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:X80"/>
+  <dimension ref="B2:X107"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14:P14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A66" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M100" sqref="M100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="68" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="68" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="68" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="68" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="68" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.5703125" style="68" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="68" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="68" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="68" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="68" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="68" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="68" customWidth="1"/>
-    <col min="15" max="16" width="11.5703125" style="68" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" style="68" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" style="68" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="68" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" style="68" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" style="68" customWidth="1"/>
-    <col min="22" max="24" width="11.5703125" style="68" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="68"/>
+    <col min="1" max="1" width="3.5" style="68" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="68" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="68" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="68" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.5" style="68" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="68" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="68" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="68" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" style="68" customWidth="1"/>
+    <col min="13" max="13" width="13.5" style="68" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="68" customWidth="1"/>
+    <col min="15" max="16" width="11.5" style="68" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" style="68" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.1640625" style="68" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" style="68" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" style="68" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" style="68" customWidth="1"/>
+    <col min="22" max="24" width="11.5" style="68" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.1640625" style="68"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:24" ht="96" x14ac:dyDescent="0.2">
       <c r="B2" s="67" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="110"/>
-      <c r="C4" s="112" t="s">
+    <row r="3" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B4" s="134"/>
+      <c r="C4" s="136" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="113"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="113"/>
-      <c r="R4" s="110"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="113"/>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="111"/>
-      <c r="C5" s="114" t="s">
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="137"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="136"/>
+      <c r="L4" s="136"/>
+      <c r="M4" s="136"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="137"/>
+      <c r="R4" s="157"/>
+      <c r="S4" s="148"/>
+      <c r="T4" s="149"/>
+      <c r="U4" s="149"/>
+      <c r="V4" s="149"/>
+      <c r="W4" s="149"/>
+      <c r="X4" s="150"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B5" s="135"/>
+      <c r="C5" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114" t="s">
+      <c r="D5" s="138"/>
+      <c r="E5" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="F5" s="138"/>
+      <c r="G5" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="H5" s="115" t="s">
+      <c r="H5" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="J5" s="111"/>
-      <c r="K5" s="114" t="s">
+      <c r="J5" s="135"/>
+      <c r="K5" s="138" t="s">
         <v>179</v>
       </c>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114" t="s">
+      <c r="L5" s="138"/>
+      <c r="M5" s="138" t="s">
         <v>181</v>
       </c>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114" t="s">
+      <c r="N5" s="138"/>
+      <c r="O5" s="153" t="s">
         <v>157</v>
       </c>
-      <c r="P5" s="115" t="s">
+      <c r="P5" s="151" t="s">
         <v>156</v>
       </c>
-      <c r="R5" s="111"/>
-      <c r="S5" s="114" t="s">
+      <c r="R5" s="158"/>
+      <c r="S5" s="146" t="s">
         <v>180</v>
       </c>
-      <c r="T5" s="114"/>
-      <c r="U5" s="114" t="s">
+      <c r="T5" s="147"/>
+      <c r="U5" s="146" t="s">
         <v>182</v>
       </c>
-      <c r="V5" s="114"/>
-      <c r="W5" s="114" t="s">
+      <c r="V5" s="147"/>
+      <c r="W5" s="153" t="s">
         <v>157</v>
       </c>
-      <c r="X5" s="115" t="s">
+      <c r="X5" s="139" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="111"/>
+    <row r="6" spans="2:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="135"/>
       <c r="C6" s="70" t="s">
         <v>6</v>
       </c>
@@ -3434,9 +3766,9 @@
       <c r="F6" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="114"/>
-      <c r="H6" s="115"/>
-      <c r="J6" s="111"/>
+      <c r="G6" s="138"/>
+      <c r="H6" s="139"/>
+      <c r="J6" s="135"/>
       <c r="K6" s="70" t="s">
         <v>6</v>
       </c>
@@ -3449,9 +3781,9 @@
       <c r="N6" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="114"/>
-      <c r="P6" s="115"/>
-      <c r="R6" s="111"/>
+      <c r="O6" s="154"/>
+      <c r="P6" s="152"/>
+      <c r="R6" s="159"/>
       <c r="S6" s="70" t="s">
         <v>6</v>
       </c>
@@ -3464,10 +3796,10 @@
       <c r="V6" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="W6" s="114"/>
-      <c r="X6" s="115"/>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="W6" s="154"/>
+      <c r="X6" s="139"/>
+    </row>
+    <row r="7" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="69" t="s">
         <v>158</v>
       </c>
@@ -3532,7 +3864,7 @@
         <v>0.80614176139159899</v>
       </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="69" t="s">
         <v>159</v>
       </c>
@@ -3597,7 +3929,7 @@
         <v>0.50799698863412102</v>
       </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="69" t="s">
         <v>113</v>
       </c>
@@ -3662,7 +3994,7 @@
         <v>2.85987048958064E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="69" t="s">
         <v>131</v>
       </c>
@@ -3727,7 +4059,7 @@
         <v>0.13017936955531401</v>
       </c>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="69" t="s">
         <v>152</v>
       </c>
@@ -3792,7 +4124,7 @@
         <v>0.53803262722269696</v>
       </c>
     </row>
-    <row r="12" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="69" t="s">
         <v>153</v>
       </c>
@@ -3857,7 +4189,7 @@
         <v>1.7608763137178698E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:24" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:24" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="78" t="s">
         <v>190</v>
       </c>
@@ -3922,7 +4254,7 @@
         <v>3.9943285088649902E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="68" t="s">
         <v>194</v>
       </c>
@@ -3987,7 +4319,7 @@
         <v>0.39372949183277101</v>
       </c>
     </row>
-    <row r="15" spans="2:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G15" s="42"/>
       <c r="H15" s="42"/>
       <c r="M15" s="42"/>
@@ -4001,7 +4333,7 @@
       <c r="W15" s="42"/>
       <c r="X15" s="42"/>
     </row>
-    <row r="16" spans="2:24" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:24" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M16" s="42"/>
       <c r="N16" s="42"/>
       <c r="S16" s="42"/>
@@ -4009,80 +4341,80 @@
       <c r="U16" s="42"/>
       <c r="V16" s="42"/>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B17" s="110"/>
-      <c r="C17" s="112" t="s">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B17" s="134"/>
+      <c r="C17" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="113"/>
-      <c r="J17" s="110"/>
-      <c r="K17" s="112"/>
-      <c r="L17" s="112"/>
-      <c r="M17" s="112"/>
-      <c r="N17" s="112"/>
-      <c r="O17" s="112"/>
-      <c r="P17" s="113"/>
-      <c r="R17" s="110"/>
-      <c r="S17" s="112"/>
-      <c r="T17" s="112"/>
-      <c r="U17" s="112"/>
-      <c r="V17" s="112"/>
-      <c r="W17" s="112"/>
-      <c r="X17" s="113"/>
-    </row>
-    <row r="18" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="111"/>
-      <c r="C18" s="114" t="s">
+      <c r="D17" s="136"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="136"/>
+      <c r="H17" s="137"/>
+      <c r="J17" s="134"/>
+      <c r="K17" s="136"/>
+      <c r="L17" s="136"/>
+      <c r="M17" s="136"/>
+      <c r="N17" s="136"/>
+      <c r="O17" s="136"/>
+      <c r="P17" s="137"/>
+      <c r="R17" s="157"/>
+      <c r="S17" s="148"/>
+      <c r="T17" s="149"/>
+      <c r="U17" s="149"/>
+      <c r="V17" s="149"/>
+      <c r="W17" s="149"/>
+      <c r="X17" s="150"/>
+    </row>
+    <row r="18" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="135"/>
+      <c r="C18" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114" t="s">
+      <c r="D18" s="138"/>
+      <c r="E18" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114" t="s">
+      <c r="F18" s="138"/>
+      <c r="G18" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="H18" s="115" t="s">
+      <c r="H18" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="J18" s="111"/>
-      <c r="K18" s="114" t="s">
+      <c r="J18" s="135"/>
+      <c r="K18" s="138" t="s">
         <v>179</v>
       </c>
-      <c r="L18" s="114"/>
-      <c r="M18" s="114" t="s">
+      <c r="L18" s="138"/>
+      <c r="M18" s="138" t="s">
         <v>180</v>
       </c>
-      <c r="N18" s="114"/>
-      <c r="O18" s="114" t="s">
+      <c r="N18" s="138"/>
+      <c r="O18" s="153" t="s">
         <v>157</v>
       </c>
-      <c r="P18" s="115" t="s">
+      <c r="P18" s="151" t="s">
         <v>156</v>
       </c>
-      <c r="R18" s="111"/>
-      <c r="S18" s="114" t="s">
+      <c r="R18" s="158"/>
+      <c r="S18" s="146" t="s">
         <v>193</v>
       </c>
-      <c r="T18" s="114"/>
-      <c r="U18" s="114" t="s">
+      <c r="T18" s="147"/>
+      <c r="U18" s="146" t="s">
         <v>182</v>
       </c>
-      <c r="V18" s="114"/>
-      <c r="W18" s="114" t="s">
+      <c r="V18" s="147"/>
+      <c r="W18" s="153" t="s">
         <v>157</v>
       </c>
-      <c r="X18" s="115" t="s">
+      <c r="X18" s="139" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="111"/>
+    <row r="19" spans="2:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="135"/>
       <c r="C19" s="70" t="s">
         <v>6</v>
       </c>
@@ -4095,9 +4427,9 @@
       <c r="F19" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="114"/>
-      <c r="H19" s="115"/>
-      <c r="J19" s="111"/>
+      <c r="G19" s="138"/>
+      <c r="H19" s="139"/>
+      <c r="J19" s="135"/>
       <c r="K19" s="70" t="s">
         <v>6</v>
       </c>
@@ -4110,9 +4442,9 @@
       <c r="N19" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="O19" s="114"/>
-      <c r="P19" s="115"/>
-      <c r="R19" s="111"/>
+      <c r="O19" s="154"/>
+      <c r="P19" s="152"/>
+      <c r="R19" s="159"/>
       <c r="S19" s="70" t="s">
         <v>6</v>
       </c>
@@ -4125,10 +4457,10 @@
       <c r="V19" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="W19" s="114"/>
-      <c r="X19" s="115"/>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="W19" s="154"/>
+      <c r="X19" s="139"/>
+    </row>
+    <row r="20" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="69" t="s">
         <v>158</v>
       </c>
@@ -4193,7 +4525,7 @@
         <v>0.79291987994251101</v>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="69" t="s">
         <v>159</v>
       </c>
@@ -4258,7 +4590,7 @@
         <v>9.6171979138577602E-4</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="69" t="s">
         <v>113</v>
       </c>
@@ -4323,7 +4655,7 @@
         <v>0.85611421505617002</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="69" t="s">
         <v>131</v>
       </c>
@@ -4388,7 +4720,7 @@
         <v>2.0477064788281501E-3</v>
       </c>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="69" t="s">
         <v>152</v>
       </c>
@@ -4453,7 +4785,7 @@
         <v>0.89276012103289504</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="69" t="s">
         <v>153</v>
       </c>
@@ -4510,7 +4842,7 @@
       <c r="W25" s="74"/>
       <c r="X25" s="75"/>
     </row>
-    <row r="26" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:24" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="78" t="s">
         <v>190</v>
       </c>
@@ -4575,7 +4907,7 @@
         <v>0.20567258764483401</v>
       </c>
     </row>
-    <row r="27" spans="2:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B27" s="68" t="s">
         <v>194</v>
       </c>
@@ -4640,7 +4972,7 @@
         <v>0.58194587052563795</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C28" s="42"/>
       <c r="D28" s="42"/>
       <c r="E28" s="42"/>
@@ -4658,54 +4990,54 @@
       <c r="W28"/>
       <c r="X28"/>
     </row>
-    <row r="29" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C29" s="42"/>
       <c r="D29" s="42"/>
       <c r="E29" s="42"/>
       <c r="F29" s="42"/>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B30" s="110"/>
-      <c r="C30" s="112" t="s">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B30" s="134"/>
+      <c r="C30" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="112"/>
-      <c r="E30" s="112"/>
-      <c r="F30" s="112"/>
-      <c r="G30" s="112"/>
-      <c r="H30" s="112"/>
-      <c r="I30" s="112"/>
-      <c r="J30" s="112"/>
-      <c r="K30" s="112"/>
-      <c r="L30" s="113"/>
-    </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B31" s="111"/>
-      <c r="C31" s="114" t="s">
+      <c r="D30" s="136"/>
+      <c r="E30" s="136"/>
+      <c r="F30" s="136"/>
+      <c r="G30" s="136"/>
+      <c r="H30" s="136"/>
+      <c r="I30" s="136"/>
+      <c r="J30" s="136"/>
+      <c r="K30" s="136"/>
+      <c r="L30" s="137"/>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B31" s="135"/>
+      <c r="C31" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114" t="s">
+      <c r="D31" s="138"/>
+      <c r="E31" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="F31" s="114"/>
-      <c r="G31" s="114" t="s">
+      <c r="F31" s="138"/>
+      <c r="G31" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="H31" s="114"/>
-      <c r="I31" s="114" t="s">
+      <c r="H31" s="138"/>
+      <c r="I31" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="J31" s="114"/>
-      <c r="K31" s="114" t="s">
+      <c r="J31" s="138"/>
+      <c r="K31" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="L31" s="115" t="s">
+      <c r="L31" s="139" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B32" s="111"/>
+    <row r="32" spans="2:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="135"/>
       <c r="C32" s="70" t="s">
         <v>6</v>
       </c>
@@ -4730,10 +5062,10 @@
       <c r="J32" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="K32" s="114"/>
-      <c r="L32" s="115"/>
-    </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="K32" s="138"/>
+      <c r="L32" s="139"/>
+    </row>
+    <row r="33" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="69" t="s">
         <v>158</v>
       </c>
@@ -4764,7 +5096,7 @@
       <c r="K33" s="71"/>
       <c r="L33" s="72"/>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="69" t="s">
         <v>159</v>
       </c>
@@ -4795,7 +5127,7 @@
       <c r="K34" s="71"/>
       <c r="L34" s="72"/>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="69" t="s">
         <v>113</v>
       </c>
@@ -4826,7 +5158,7 @@
       <c r="K35" s="71"/>
       <c r="L35" s="72"/>
     </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="69" t="s">
         <v>131</v>
       </c>
@@ -4857,7 +5189,7 @@
       <c r="K36" s="71"/>
       <c r="L36" s="72"/>
     </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="69" t="s">
         <v>152</v>
       </c>
@@ -4888,7 +5220,7 @@
       <c r="K37" s="71"/>
       <c r="L37" s="72"/>
     </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="69" t="s">
         <v>153</v>
       </c>
@@ -4919,7 +5251,7 @@
       <c r="K38" s="71"/>
       <c r="L38" s="72"/>
     </row>
-    <row r="39" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:24" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="78" t="s">
         <v>190</v>
       </c>
@@ -4950,7 +5282,7 @@
       <c r="K39" s="79"/>
       <c r="L39" s="84"/>
     </row>
-    <row r="40" spans="2:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B40" s="68" t="s">
         <v>194</v>
       </c>
@@ -4979,7 +5311,7 @@
         <v>0.22148394241417399</v>
       </c>
     </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C41" s="42"/>
       <c r="D41" s="42"/>
       <c r="E41" s="42"/>
@@ -4989,7 +5321,7 @@
       <c r="I41" s="42"/>
       <c r="J41" s="42"/>
     </row>
-    <row r="42" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C42" s="42"/>
       <c r="D42" s="42"/>
       <c r="E42" s="42"/>
@@ -4999,84 +5331,84 @@
       <c r="I42" s="42"/>
       <c r="J42" s="42"/>
     </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B43" s="110"/>
-      <c r="C43" s="112" t="s">
+    <row r="43" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B43" s="134"/>
+      <c r="C43" s="136" t="s">
         <v>177</v>
       </c>
-      <c r="D43" s="112"/>
-      <c r="E43" s="112"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="112"/>
-      <c r="H43" s="112"/>
-      <c r="I43" s="112"/>
-      <c r="J43" s="112"/>
-      <c r="K43" s="112"/>
-      <c r="L43" s="113"/>
-      <c r="N43" s="110"/>
-      <c r="O43" s="112" t="s">
+      <c r="D43" s="136"/>
+      <c r="E43" s="136"/>
+      <c r="F43" s="136"/>
+      <c r="G43" s="136"/>
+      <c r="H43" s="136"/>
+      <c r="I43" s="136"/>
+      <c r="J43" s="136"/>
+      <c r="K43" s="136"/>
+      <c r="L43" s="137"/>
+      <c r="N43" s="134"/>
+      <c r="O43" s="148" t="s">
         <v>178</v>
       </c>
-      <c r="P43" s="112"/>
-      <c r="Q43" s="112"/>
-      <c r="R43" s="112"/>
-      <c r="S43" s="112"/>
-      <c r="T43" s="112"/>
-      <c r="U43" s="112"/>
-      <c r="V43" s="112"/>
-      <c r="W43" s="112"/>
-      <c r="X43" s="113"/>
-    </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B44" s="111"/>
-      <c r="C44" s="114" t="s">
+      <c r="P43" s="149"/>
+      <c r="Q43" s="149"/>
+      <c r="R43" s="149"/>
+      <c r="S43" s="149"/>
+      <c r="T43" s="149"/>
+      <c r="U43" s="149"/>
+      <c r="V43" s="149"/>
+      <c r="W43" s="149"/>
+      <c r="X43" s="150"/>
+    </row>
+    <row r="44" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B44" s="135"/>
+      <c r="C44" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="114"/>
-      <c r="E44" s="114" t="s">
+      <c r="D44" s="138"/>
+      <c r="E44" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="F44" s="114"/>
-      <c r="G44" s="114" t="s">
+      <c r="F44" s="138"/>
+      <c r="G44" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="H44" s="114"/>
-      <c r="I44" s="114" t="s">
+      <c r="H44" s="138"/>
+      <c r="I44" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="J44" s="114"/>
-      <c r="K44" s="114" t="s">
+      <c r="J44" s="138"/>
+      <c r="K44" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="L44" s="115" t="s">
+      <c r="L44" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="N44" s="111"/>
-      <c r="O44" s="114" t="s">
+      <c r="N44" s="135"/>
+      <c r="O44" s="146" t="s">
         <v>106</v>
       </c>
-      <c r="P44" s="114"/>
-      <c r="Q44" s="114" t="s">
+      <c r="P44" s="147"/>
+      <c r="Q44" s="146" t="s">
         <v>167</v>
       </c>
-      <c r="R44" s="114"/>
-      <c r="S44" s="114" t="s">
+      <c r="R44" s="147"/>
+      <c r="S44" s="146" t="s">
         <v>108</v>
       </c>
-      <c r="T44" s="114"/>
-      <c r="U44" s="114" t="s">
+      <c r="T44" s="147"/>
+      <c r="U44" s="146" t="s">
         <v>168</v>
       </c>
-      <c r="V44" s="114"/>
-      <c r="W44" s="114" t="s">
+      <c r="V44" s="147"/>
+      <c r="W44" s="153" t="s">
         <v>157</v>
       </c>
-      <c r="X44" s="115" t="s">
+      <c r="X44" s="139" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B45" s="111"/>
+    <row r="45" spans="2:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="B45" s="135"/>
       <c r="C45" s="70" t="s">
         <v>6</v>
       </c>
@@ -5101,9 +5433,9 @@
       <c r="J45" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="K45" s="114"/>
-      <c r="L45" s="115"/>
-      <c r="N45" s="111"/>
+      <c r="K45" s="138"/>
+      <c r="L45" s="139"/>
+      <c r="N45" s="135"/>
       <c r="O45" s="70" t="s">
         <v>6</v>
       </c>
@@ -5128,10 +5460,10 @@
       <c r="V45" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="W45" s="114"/>
-      <c r="X45" s="115"/>
-    </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="W45" s="154"/>
+      <c r="X45" s="139"/>
+    </row>
+    <row r="46" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="69" t="s">
         <v>158</v>
       </c>
@@ -5191,7 +5523,7 @@
       <c r="W46" s="71"/>
       <c r="X46" s="72"/>
     </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="69" t="s">
         <v>159</v>
       </c>
@@ -5251,7 +5583,7 @@
       <c r="W47" s="71"/>
       <c r="X47" s="72"/>
     </row>
-    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="69" t="s">
         <v>113</v>
       </c>
@@ -5311,7 +5643,7 @@
       <c r="W48" s="71"/>
       <c r="X48" s="72"/>
     </row>
-    <row r="49" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="69" t="s">
         <v>131</v>
       </c>
@@ -5371,7 +5703,7 @@
       <c r="W49" s="71"/>
       <c r="X49" s="72"/>
     </row>
-    <row r="50" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="69" t="s">
         <v>152</v>
       </c>
@@ -5431,7 +5763,7 @@
       <c r="W50" s="71"/>
       <c r="X50" s="72"/>
     </row>
-    <row r="51" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="69" t="s">
         <v>153</v>
       </c>
@@ -5491,7 +5823,7 @@
       <c r="W51" s="71"/>
       <c r="X51" s="72"/>
     </row>
-    <row r="52" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:24" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="78" t="s">
         <v>190</v>
       </c>
@@ -5551,7 +5883,7 @@
       <c r="W52" s="79"/>
       <c r="X52" s="84"/>
     </row>
-    <row r="53" spans="2:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B53" s="68" t="s">
         <v>194</v>
       </c>
@@ -5607,7 +5939,7 @@
         <v>0.26809651474530799</v>
       </c>
     </row>
-    <row r="54" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
       <c r="E54" s="42"/>
@@ -5625,85 +5957,85 @@
       <c r="U54" s="42"/>
       <c r="V54" s="42"/>
     </row>
-    <row r="55" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B56" s="110"/>
-      <c r="C56" s="112" t="s">
+    <row r="55" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B56" s="134"/>
+      <c r="C56" s="136" t="s">
         <v>184</v>
       </c>
-      <c r="D56" s="112"/>
-      <c r="E56" s="112"/>
-      <c r="F56" s="112"/>
-      <c r="G56" s="112"/>
-      <c r="H56" s="112"/>
-      <c r="I56" s="112"/>
-      <c r="J56" s="112"/>
-      <c r="K56" s="112"/>
-      <c r="L56" s="113"/>
-      <c r="N56" s="110"/>
-      <c r="O56" s="112" t="s">
+      <c r="D56" s="136"/>
+      <c r="E56" s="136"/>
+      <c r="F56" s="136"/>
+      <c r="G56" s="136"/>
+      <c r="H56" s="136"/>
+      <c r="I56" s="136"/>
+      <c r="J56" s="136"/>
+      <c r="K56" s="136"/>
+      <c r="L56" s="137"/>
+      <c r="N56" s="134"/>
+      <c r="O56" s="148" t="s">
         <v>197</v>
       </c>
-      <c r="P56" s="112"/>
-      <c r="Q56" s="112"/>
-      <c r="R56" s="112"/>
-      <c r="S56" s="112"/>
-      <c r="T56" s="112"/>
-      <c r="U56" s="112"/>
-      <c r="V56" s="112"/>
-      <c r="W56" s="112"/>
-      <c r="X56" s="113"/>
-    </row>
-    <row r="57" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B57" s="111"/>
-      <c r="C57" s="114" t="s">
+      <c r="P56" s="149"/>
+      <c r="Q56" s="149"/>
+      <c r="R56" s="149"/>
+      <c r="S56" s="149"/>
+      <c r="T56" s="149"/>
+      <c r="U56" s="149"/>
+      <c r="V56" s="149"/>
+      <c r="W56" s="149"/>
+      <c r="X56" s="150"/>
+    </row>
+    <row r="57" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B57" s="135"/>
+      <c r="C57" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="114"/>
-      <c r="E57" s="114" t="s">
+      <c r="D57" s="138"/>
+      <c r="E57" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="F57" s="114"/>
-      <c r="G57" s="114" t="s">
+      <c r="F57" s="138"/>
+      <c r="G57" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="H57" s="114"/>
-      <c r="I57" s="114" t="s">
+      <c r="H57" s="138"/>
+      <c r="I57" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="J57" s="114"/>
-      <c r="K57" s="114" t="s">
+      <c r="J57" s="138"/>
+      <c r="K57" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="L57" s="115" t="s">
+      <c r="L57" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="N57" s="111"/>
-      <c r="O57" s="114" t="s">
+      <c r="N57" s="135"/>
+      <c r="O57" s="146" t="s">
         <v>106</v>
       </c>
-      <c r="P57" s="114"/>
-      <c r="Q57" s="114" t="s">
+      <c r="P57" s="147"/>
+      <c r="Q57" s="146" t="s">
         <v>167</v>
       </c>
-      <c r="R57" s="114"/>
-      <c r="S57" s="114" t="s">
+      <c r="R57" s="147"/>
+      <c r="S57" s="146" t="s">
         <v>108</v>
       </c>
-      <c r="T57" s="114"/>
-      <c r="U57" s="114" t="s">
+      <c r="T57" s="147"/>
+      <c r="U57" s="146" t="s">
         <v>168</v>
       </c>
-      <c r="V57" s="114"/>
-      <c r="W57" s="114" t="s">
+      <c r="V57" s="147"/>
+      <c r="W57" s="153" t="s">
         <v>157</v>
       </c>
-      <c r="X57" s="115" t="s">
+      <c r="X57" s="139" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B58" s="111"/>
+    <row r="58" spans="2:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="B58" s="135"/>
       <c r="C58" s="70" t="s">
         <v>6</v>
       </c>
@@ -5728,9 +6060,9 @@
       <c r="J58" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="K58" s="114"/>
-      <c r="L58" s="115"/>
-      <c r="N58" s="111"/>
+      <c r="K58" s="138"/>
+      <c r="L58" s="139"/>
+      <c r="N58" s="135"/>
       <c r="O58" s="70" t="s">
         <v>6</v>
       </c>
@@ -5755,10 +6087,10 @@
       <c r="V58" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="W58" s="114"/>
-      <c r="X58" s="115"/>
-    </row>
-    <row r="59" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="W58" s="154"/>
+      <c r="X58" s="139"/>
+    </row>
+    <row r="59" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="69" t="s">
         <v>158</v>
       </c>
@@ -5818,7 +6150,7 @@
       <c r="W59" s="71"/>
       <c r="X59" s="72"/>
     </row>
-    <row r="60" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B60" s="69" t="s">
         <v>159</v>
       </c>
@@ -5878,7 +6210,7 @@
       <c r="W60" s="71"/>
       <c r="X60" s="72"/>
     </row>
-    <row r="61" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B61" s="69" t="s">
         <v>113</v>
       </c>
@@ -5938,7 +6270,7 @@
       <c r="W61" s="71"/>
       <c r="X61" s="72"/>
     </row>
-    <row r="62" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B62" s="69" t="s">
         <v>131</v>
       </c>
@@ -5998,7 +6330,7 @@
       <c r="W62" s="71"/>
       <c r="X62" s="72"/>
     </row>
-    <row r="63" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" s="69" t="s">
         <v>152</v>
       </c>
@@ -6058,7 +6390,7 @@
       <c r="W63" s="71"/>
       <c r="X63" s="72"/>
     </row>
-    <row r="64" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B64" s="69" t="s">
         <v>153</v>
       </c>
@@ -6118,7 +6450,7 @@
       <c r="W64" s="71"/>
       <c r="X64" s="72"/>
     </row>
-    <row r="65" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:24" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B65" s="78" t="s">
         <v>190</v>
       </c>
@@ -6178,7 +6510,7 @@
       <c r="W65" s="79"/>
       <c r="X65" s="84"/>
     </row>
-    <row r="66" spans="2:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B66" s="68" t="s">
         <v>194</v>
       </c>
@@ -6234,7 +6566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C67" s="42"/>
       <c r="D67" s="42"/>
       <c r="E67" s="42"/>
@@ -6252,87 +6584,87 @@
       <c r="U67" s="42"/>
       <c r="V67" s="42"/>
     </row>
-    <row r="68" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F68" s="67"/>
     </row>
-    <row r="69" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B69" s="110"/>
-      <c r="C69" s="112" t="s">
+    <row r="69" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B69" s="134"/>
+      <c r="C69" s="136" t="s">
         <v>196</v>
       </c>
-      <c r="D69" s="112"/>
-      <c r="E69" s="112"/>
-      <c r="F69" s="112"/>
-      <c r="G69" s="112"/>
-      <c r="H69" s="112"/>
-      <c r="I69" s="112"/>
-      <c r="J69" s="112"/>
-      <c r="K69" s="112"/>
-      <c r="L69" s="113"/>
-      <c r="N69" s="110"/>
-      <c r="O69" s="112" t="s">
+      <c r="D69" s="136"/>
+      <c r="E69" s="136"/>
+      <c r="F69" s="136"/>
+      <c r="G69" s="136"/>
+      <c r="H69" s="136"/>
+      <c r="I69" s="136"/>
+      <c r="J69" s="136"/>
+      <c r="K69" s="136"/>
+      <c r="L69" s="137"/>
+      <c r="N69" s="134"/>
+      <c r="O69" s="148" t="s">
         <v>195</v>
       </c>
-      <c r="P69" s="112"/>
-      <c r="Q69" s="112"/>
-      <c r="R69" s="112"/>
-      <c r="S69" s="112"/>
-      <c r="T69" s="112"/>
-      <c r="U69" s="112"/>
-      <c r="V69" s="112"/>
-      <c r="W69" s="112"/>
-      <c r="X69" s="113"/>
-    </row>
-    <row r="70" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B70" s="111"/>
-      <c r="C70" s="114" t="s">
+      <c r="P69" s="149"/>
+      <c r="Q69" s="149"/>
+      <c r="R69" s="149"/>
+      <c r="S69" s="149"/>
+      <c r="T69" s="149"/>
+      <c r="U69" s="149"/>
+      <c r="V69" s="149"/>
+      <c r="W69" s="149"/>
+      <c r="X69" s="150"/>
+    </row>
+    <row r="70" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B70" s="135"/>
+      <c r="C70" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="D70" s="114"/>
-      <c r="E70" s="114" t="s">
+      <c r="D70" s="138"/>
+      <c r="E70" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="F70" s="114"/>
-      <c r="G70" s="114" t="s">
+      <c r="F70" s="138"/>
+      <c r="G70" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="H70" s="114"/>
-      <c r="I70" s="114" t="s">
+      <c r="H70" s="138"/>
+      <c r="I70" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="J70" s="114"/>
-      <c r="K70" s="114" t="s">
+      <c r="J70" s="138"/>
+      <c r="K70" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="L70" s="115" t="s">
+      <c r="L70" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="N70" s="111"/>
-      <c r="O70" s="114" t="s">
+      <c r="N70" s="135"/>
+      <c r="O70" s="146" t="s">
         <v>106</v>
       </c>
-      <c r="P70" s="114"/>
-      <c r="Q70" s="114" t="s">
+      <c r="P70" s="147"/>
+      <c r="Q70" s="146" t="s">
         <v>167</v>
       </c>
-      <c r="R70" s="114"/>
-      <c r="S70" s="114" t="s">
+      <c r="R70" s="147"/>
+      <c r="S70" s="146" t="s">
         <v>108</v>
       </c>
-      <c r="T70" s="114"/>
-      <c r="U70" s="114" t="s">
+      <c r="T70" s="147"/>
+      <c r="U70" s="146" t="s">
         <v>168</v>
       </c>
-      <c r="V70" s="114"/>
-      <c r="W70" s="114" t="s">
+      <c r="V70" s="147"/>
+      <c r="W70" s="153" t="s">
         <v>157</v>
       </c>
-      <c r="X70" s="115" t="s">
+      <c r="X70" s="139" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B71" s="111"/>
+    <row r="71" spans="2:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="B71" s="135"/>
       <c r="C71" s="70" t="s">
         <v>6</v>
       </c>
@@ -6357,9 +6689,9 @@
       <c r="J71" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="K71" s="114"/>
-      <c r="L71" s="115"/>
-      <c r="N71" s="111"/>
+      <c r="K71" s="138"/>
+      <c r="L71" s="139"/>
+      <c r="N71" s="135"/>
       <c r="O71" s="70" t="s">
         <v>6</v>
       </c>
@@ -6384,10 +6716,10 @@
       <c r="V71" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="W71" s="114"/>
-      <c r="X71" s="115"/>
-    </row>
-    <row r="72" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="W71" s="154"/>
+      <c r="X71" s="139"/>
+    </row>
+    <row r="72" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="69" t="s">
         <v>158</v>
       </c>
@@ -6447,7 +6779,7 @@
       <c r="W72" s="71"/>
       <c r="X72" s="72"/>
     </row>
-    <row r="73" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B73" s="69" t="s">
         <v>159</v>
       </c>
@@ -6507,7 +6839,7 @@
       <c r="W73" s="71"/>
       <c r="X73" s="72"/>
     </row>
-    <row r="74" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B74" s="69" t="s">
         <v>113</v>
       </c>
@@ -6567,7 +6899,7 @@
       <c r="W74" s="71"/>
       <c r="X74" s="72"/>
     </row>
-    <row r="75" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" s="69" t="s">
         <v>131</v>
       </c>
@@ -6627,7 +6959,7 @@
       <c r="W75" s="71"/>
       <c r="X75" s="72"/>
     </row>
-    <row r="76" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B76" s="69" t="s">
         <v>152</v>
       </c>
@@ -6687,7 +7019,7 @@
       <c r="W76" s="71"/>
       <c r="X76" s="72"/>
     </row>
-    <row r="77" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B77" s="69" t="s">
         <v>153</v>
       </c>
@@ -6747,7 +7079,7 @@
       <c r="W77" s="71"/>
       <c r="X77" s="72"/>
     </row>
-    <row r="78" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:24" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="69" t="s">
         <v>190</v>
       </c>
@@ -6807,7 +7139,7 @@
       <c r="W78" s="79"/>
       <c r="X78" s="84"/>
     </row>
-    <row r="79" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:24" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B79" s="78"/>
       <c r="C79" s="79"/>
       <c r="D79" s="79"/>
@@ -6847,7 +7179,7 @@
         <v>0.16963528413910001</v>
       </c>
     </row>
-    <row r="80" spans="2:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B80" s="68" t="s">
         <v>194</v>
       </c>
@@ -6876,8 +7208,434 @@
         <v>0.65789473684210498</v>
       </c>
     </row>
+    <row r="85" spans="6:21" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="6:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O86" s="157"/>
+      <c r="P86" s="148" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q86" s="149"/>
+      <c r="R86" s="149"/>
+      <c r="S86" s="149"/>
+      <c r="T86" s="155"/>
+      <c r="U86" s="156"/>
+    </row>
+    <row r="87" spans="6:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F87"/>
+      <c r="G87"/>
+      <c r="H87"/>
+      <c r="O87" s="158"/>
+      <c r="P87" s="146" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q87" s="147"/>
+      <c r="R87" s="146" t="s">
+        <v>203</v>
+      </c>
+      <c r="S87" s="147"/>
+      <c r="T87" s="153" t="s">
+        <v>157</v>
+      </c>
+      <c r="U87" s="151" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="88" spans="6:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="O88" s="159"/>
+      <c r="P88" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q88" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="R88" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="S88" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="T88" s="154"/>
+      <c r="U88" s="152"/>
+    </row>
+    <row r="89" spans="6:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="O89" s="69" t="s">
+        <v>158</v>
+      </c>
+      <c r="P89" s="145">
+        <v>832</v>
+      </c>
+      <c r="Q89" s="145">
+        <v>41.3930348258706</v>
+      </c>
+      <c r="R89" s="46">
+        <v>3761</v>
+      </c>
+      <c r="S89" s="46">
+        <v>44.096611560558003</v>
+      </c>
+      <c r="T89" s="46">
+        <v>0.89538733918705404</v>
+      </c>
+      <c r="U89" s="46">
+        <v>2.78304138476059E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="6:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="O90" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="P90" s="145">
+        <v>374</v>
+      </c>
+      <c r="Q90" s="145">
+        <v>18.6069651741293</v>
+      </c>
+      <c r="R90" s="46">
+        <v>1624</v>
+      </c>
+      <c r="S90" s="46">
+        <v>19.0409192167897</v>
+      </c>
+      <c r="T90" s="46">
+        <v>0.97199931949847596</v>
+      </c>
+      <c r="U90" s="46">
+        <v>0.68095921289037598</v>
+      </c>
+    </row>
+    <row r="91" spans="6:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="F91"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="O91" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="P91" s="145">
+        <v>221</v>
+      </c>
+      <c r="Q91" s="145">
+        <v>10.9950248756218</v>
+      </c>
+      <c r="R91" s="46">
+        <v>958</v>
+      </c>
+      <c r="S91" s="46">
+        <v>11.2322663852737</v>
+      </c>
+      <c r="T91" s="46">
+        <v>0.97626938458288903</v>
+      </c>
+      <c r="U91" s="46">
+        <v>0.78315782838171699</v>
+      </c>
+    </row>
+    <row r="92" spans="6:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="F92"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="O92" s="69" t="s">
+        <v>131</v>
+      </c>
+      <c r="P92" s="145">
+        <v>506</v>
+      </c>
+      <c r="Q92" s="145">
+        <v>25.174129353233798</v>
+      </c>
+      <c r="R92" s="46">
+        <v>1819</v>
+      </c>
+      <c r="S92" s="46">
+        <v>21.327236487278601</v>
+      </c>
+      <c r="T92" s="46">
+        <v>1.2410592095259201</v>
+      </c>
+      <c r="U92" s="46">
+        <v>2.33476535897229E-4</v>
+      </c>
+    </row>
+    <row r="93" spans="6:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="O93" s="69" t="s">
+        <v>152</v>
+      </c>
+      <c r="P93" s="145">
+        <v>23</v>
+      </c>
+      <c r="Q93" s="145">
+        <v>1.14427860696517</v>
+      </c>
+      <c r="R93" s="46">
+        <v>103</v>
+      </c>
+      <c r="S93" s="46">
+        <v>1.2076445069761901</v>
+      </c>
+      <c r="T93" s="46">
+        <v>0.94692198318194398</v>
+      </c>
+      <c r="U93" s="46">
+        <v>0.90927803347041802</v>
+      </c>
+    </row>
+    <row r="94" spans="6:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="O94" s="69" t="s">
+        <v>153</v>
+      </c>
+      <c r="P94" s="145">
+        <v>44</v>
+      </c>
+      <c r="Q94" s="145">
+        <v>2.1890547263681501</v>
+      </c>
+      <c r="R94" s="46">
+        <v>212</v>
+      </c>
+      <c r="S94" s="46">
+        <v>2.48563723765974</v>
+      </c>
+      <c r="T94" s="46">
+        <v>0.87801109426284496</v>
+      </c>
+      <c r="U94" s="46">
+        <v>0.46933067221630598</v>
+      </c>
+    </row>
+    <row r="95" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="O95" s="69"/>
+      <c r="P95" s="145"/>
+      <c r="Q95" s="145"/>
+      <c r="R95" s="46">
+        <v>52</v>
+      </c>
+      <c r="S95" s="46">
+        <v>0.60968460546371195</v>
+      </c>
+      <c r="T95" s="71"/>
+      <c r="U95" s="72"/>
+    </row>
+    <row r="97" spans="15:21" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="15:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O98" s="167"/>
+      <c r="P98" s="179" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q98" s="178"/>
+      <c r="R98" s="178"/>
+      <c r="S98" s="178"/>
+      <c r="T98" s="160"/>
+      <c r="U98" s="161"/>
+    </row>
+    <row r="99" spans="15:21" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O99" s="168"/>
+      <c r="P99" s="170" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q99" s="171"/>
+      <c r="R99" s="172" t="s">
+        <v>204</v>
+      </c>
+      <c r="S99" s="173"/>
+      <c r="T99" s="175" t="s">
+        <v>157</v>
+      </c>
+      <c r="U99" s="177" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="100" spans="15:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="O100" s="169"/>
+      <c r="P100" s="162" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q100" s="162" t="s">
+        <v>7</v>
+      </c>
+      <c r="R100" s="162" t="s">
+        <v>6</v>
+      </c>
+      <c r="S100" s="162" t="s">
+        <v>7</v>
+      </c>
+      <c r="T100" s="174"/>
+      <c r="U100" s="176"/>
+    </row>
+    <row r="101" spans="15:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="O101" s="163" t="s">
+        <v>158</v>
+      </c>
+      <c r="P101" s="164">
+        <v>832</v>
+      </c>
+      <c r="Q101" s="164">
+        <v>41.393030000000003</v>
+      </c>
+      <c r="R101" s="46">
+        <v>3001</v>
+      </c>
+      <c r="S101" s="46">
+        <v>44.637810501264298</v>
+      </c>
+      <c r="T101" s="46">
+        <v>0.87596833879368996</v>
+      </c>
+      <c r="U101" s="46">
+        <v>1.0421978151965499E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="15:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="O102" s="163" t="s">
+        <v>159</v>
+      </c>
+      <c r="P102" s="164">
+        <v>374</v>
+      </c>
+      <c r="Q102" s="164">
+        <v>18.60697</v>
+      </c>
+      <c r="R102" s="46">
+        <v>1267</v>
+      </c>
+      <c r="S102" s="46">
+        <v>18.845753383905901</v>
+      </c>
+      <c r="T102" s="46">
+        <v>0.98443274160898298</v>
+      </c>
+      <c r="U102" s="46">
+        <v>0.81990985746780798</v>
+      </c>
+    </row>
+    <row r="103" spans="15:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="O103" s="163" t="s">
+        <v>113</v>
+      </c>
+      <c r="P103" s="164">
+        <v>221</v>
+      </c>
+      <c r="Q103" s="164">
+        <v>10.99502</v>
+      </c>
+      <c r="R103" s="46">
+        <v>745</v>
+      </c>
+      <c r="S103" s="46">
+        <v>11.081362486984901</v>
+      </c>
+      <c r="T103" s="46">
+        <v>0.99124628133897996</v>
+      </c>
+      <c r="U103" s="46">
+        <v>0.93543130332291202</v>
+      </c>
+    </row>
+    <row r="104" spans="15:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="O104" s="163" t="s">
+        <v>131</v>
+      </c>
+      <c r="P104" s="164">
+        <v>506</v>
+      </c>
+      <c r="Q104" s="164">
+        <v>25.174130000000002</v>
+      </c>
+      <c r="R104" s="46">
+        <v>1411</v>
+      </c>
+      <c r="S104" s="46">
+        <v>20.987654320987598</v>
+      </c>
+      <c r="T104" s="46">
+        <v>1.2665832290362899</v>
+      </c>
+      <c r="U104" s="180">
+        <v>8.0000000000000007E-5</v>
+      </c>
+    </row>
+    <row r="105" spans="15:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="O105" s="163" t="s">
+        <v>152</v>
+      </c>
+      <c r="P105" s="164">
+        <v>23</v>
+      </c>
+      <c r="Q105" s="164">
+        <v>1.144279</v>
+      </c>
+      <c r="R105" s="46">
+        <v>81</v>
+      </c>
+      <c r="S105" s="46">
+        <v>1.2048192771084301</v>
+      </c>
+      <c r="T105" s="46">
+        <v>0.94916960241570203</v>
+      </c>
+      <c r="U105" s="46">
+        <v>0.90694872373262603</v>
+      </c>
+    </row>
+    <row r="106" spans="15:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="O106" s="163" t="s">
+        <v>153</v>
+      </c>
+      <c r="P106" s="164">
+        <v>44</v>
+      </c>
+      <c r="Q106" s="164">
+        <v>2.1890550000000002</v>
+      </c>
+      <c r="R106" s="46">
+        <v>170</v>
+      </c>
+      <c r="S106" s="46">
+        <v>2.5286330507214001</v>
+      </c>
+      <c r="T106" s="46">
+        <v>0.86270121476871497</v>
+      </c>
+      <c r="U106" s="46">
+        <v>0.41201192454214303</v>
+      </c>
+    </row>
+    <row r="107" spans="15:21" x14ac:dyDescent="0.2">
+      <c r="O107" s="163"/>
+      <c r="P107" s="164"/>
+      <c r="Q107" s="164"/>
+      <c r="R107" s="164"/>
+      <c r="S107" s="164"/>
+      <c r="T107" s="165"/>
+      <c r="U107" s="166"/>
+    </row>
   </sheetData>
-  <mergeCells count="92">
+  <mergeCells count="104">
+    <mergeCell ref="O98:O100"/>
+    <mergeCell ref="P99:Q99"/>
+    <mergeCell ref="R99:S99"/>
+    <mergeCell ref="T99:T100"/>
+    <mergeCell ref="U99:U100"/>
+    <mergeCell ref="P98:S98"/>
+    <mergeCell ref="O86:O88"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="R87:S87"/>
+    <mergeCell ref="T87:T88"/>
+    <mergeCell ref="U87:U88"/>
+    <mergeCell ref="P86:S86"/>
     <mergeCell ref="B69:B71"/>
     <mergeCell ref="C69:L69"/>
     <mergeCell ref="N69:N71"/>
@@ -6984,18 +7742,18 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2:D21"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -7015,7 +7773,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
@@ -7035,7 +7793,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -7055,7 +7813,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -7075,7 +7833,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -7093,7 +7851,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -7111,7 +7869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -7125,9 +7883,11 @@
         <v>137</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -7143,7 +7903,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -7159,7 +7919,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -7175,7 +7935,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -7191,7 +7951,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -7207,7 +7967,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -7223,7 +7983,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -7237,7 +7997,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -7251,7 +8011,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -7265,7 +8025,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -7279,7 +8039,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -7293,7 +8053,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -7307,7 +8067,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
@@ -7321,7 +8081,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
@@ -7335,7 +8095,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
@@ -7347,7 +8107,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
@@ -7359,7 +8119,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -7371,7 +8131,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -7383,7 +8143,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>56</v>
       </c>
@@ -7395,7 +8155,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
@@ -7407,7 +8167,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -7419,7 +8179,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -7431,7 +8191,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>64</v>
       </c>
@@ -7443,7 +8203,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>66</v>
       </c>
@@ -7455,7 +8215,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
@@ -7467,7 +8227,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>69</v>
       </c>
@@ -7479,7 +8239,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
@@ -7491,7 +8251,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -7503,7 +8263,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
@@ -7515,7 +8275,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -7527,7 +8287,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -7539,7 +8299,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
@@ -7551,7 +8311,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>83</v>
       </c>
@@ -7563,7 +8323,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -7575,7 +8335,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>87</v>
       </c>
@@ -7587,7 +8347,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
@@ -7599,7 +8359,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>90</v>
       </c>
@@ -7611,7 +8371,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
@@ -7623,7 +8383,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>94</v>
       </c>
@@ -7635,7 +8395,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>96</v>
       </c>
@@ -7645,7 +8405,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>97</v>
       </c>
@@ -7655,7 +8415,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>98</v>
       </c>
@@ -7665,7 +8425,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
@@ -7675,7 +8435,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>100</v>
       </c>
@@ -7685,12 +8445,12 @@
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I54" s="10" t="s">
         <v>110</v>
       </c>
@@ -7714,13 +8474,13 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>130</v>
       </c>
@@ -7731,7 +8491,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C3" s="10" t="s">
         <v>103</v>
       </c>
@@ -7739,7 +8499,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C4" s="10" t="s">
         <v>104</v>
       </c>
@@ -7747,7 +8507,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>127</v>
       </c>
@@ -7758,7 +8518,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>161</v>
       </c>
@@ -7791,74 +8551,74 @@
       <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="25" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="97"/>
-      <c r="C4" s="100" t="s">
+    <row r="3" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B4" s="111"/>
+      <c r="C4" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="116" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="102" t="s">
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="103" t="s">
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="103"/>
-      <c r="N4" s="103"/>
-      <c r="O4" s="105"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="98"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="106" t="s">
+      <c r="M4" s="117"/>
+      <c r="N4" s="117"/>
+      <c r="O4" s="119"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B5" s="112"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="107"/>
-      <c r="F5" s="91" t="s">
+      <c r="E5" s="121"/>
+      <c r="F5" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="108"/>
-      <c r="H5" s="106" t="s">
+      <c r="G5" s="123"/>
+      <c r="H5" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="91" t="s">
+      <c r="I5" s="121"/>
+      <c r="J5" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="108"/>
-      <c r="L5" s="109" t="s">
+      <c r="K5" s="123"/>
+      <c r="L5" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="107"/>
-      <c r="N5" s="91" t="s">
+      <c r="M5" s="121"/>
+      <c r="N5" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="92"/>
-    </row>
-    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="99"/>
+      <c r="O5" s="129"/>
+    </row>
+    <row r="6" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="113"/>
       <c r="C6" s="37" t="s">
         <v>6</v>
       </c>
@@ -7899,7 +8659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="27" t="s">
         <v>174</v>
       </c>
@@ -7935,7 +8695,7 @@
         <v>71.726190476190396</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="27" t="s">
         <v>173</v>
       </c>
@@ -7971,7 +8731,7 @@
         <v>71.525096525096501</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
@@ -7989,7 +8749,7 @@
       <c r="N9" s="15"/>
       <c r="O9" s="18"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="23" t="s">
         <v>175</v>
       </c>
@@ -8025,7 +8785,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="23" t="s">
         <v>172</v>
       </c>
@@ -8061,7 +8821,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
         <v>10</v>
       </c>
@@ -8097,7 +8857,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="22" t="s">
         <v>11</v>
       </c>
@@ -8115,7 +8875,7 @@
       <c r="N13" s="15"/>
       <c r="O13" s="18"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
         <v>1</v>
       </c>
@@ -8151,7 +8911,7 @@
         <v>80.303030303030297</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>0</v>
       </c>
@@ -8187,7 +8947,7 @@
         <v>69.296116504854297</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="22" t="s">
         <v>12</v>
       </c>
@@ -8205,7 +8965,7 @@
       <c r="N16" s="15"/>
       <c r="O16" s="18"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
         <v>106</v>
       </c>
@@ -8243,7 +9003,7 @@
         <v>67.875647668393697</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18" s="23" t="s">
         <v>107</v>
       </c>
@@ -8281,7 +9041,7 @@
         <v>78.735632183907995</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
         <v>108</v>
       </c>
@@ -8319,7 +9079,7 @@
         <v>76.923076923076906</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>109</v>
       </c>
@@ -8357,32 +9117,32 @@
         <v>66.978922716627594</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="118" t="s">
+    <row r="21" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="142" t="s">
         <v>188</v>
       </c>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="120"/>
+      <c r="D22" s="143"/>
+      <c r="E22" s="143"/>
+      <c r="F22" s="143"/>
+      <c r="G22" s="144"/>
       <c r="H22" s="61"/>
     </row>
-    <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="116" t="s">
+    <row r="23" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="117"/>
-      <c r="E23" s="117" t="s">
+      <c r="D23" s="141"/>
+      <c r="E23" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="117"/>
+      <c r="F23" s="141"/>
       <c r="G23" s="43" t="s">
         <v>187</v>
       </c>
       <c r="H23" s="65"/>
     </row>
-    <row r="24" spans="2:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="51"/>
       <c r="C24" s="55" t="s">
         <v>6</v>
@@ -8405,7 +9165,7 @@
       <c r="O24" s="35"/>
       <c r="P24" s="35"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="52" t="s">
         <v>106</v>
       </c>
@@ -8431,7 +9191,7 @@
         <v>0.18324607329842932</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26" s="52" t="s">
         <v>107</v>
       </c>
@@ -8457,7 +9217,7 @@
         <v>0.19653179190751446</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27" s="52" t="s">
         <v>108</v>
       </c>
@@ -8483,7 +9243,7 @@
         <v>0.25217391304347825</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28" s="53" t="s">
         <v>109</v>
       </c>
@@ -8506,7 +9266,7 @@
       </c>
       <c r="H28" s="63"/>
     </row>
-    <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="54" t="s">
         <v>185</v>
       </c>

</xml_diff>